<commit_message>
update NONE icons on cards
</commit_message>
<xml_diff>
--- a/choice_cards/card_database.xlsx
+++ b/choice_cards/card_database.xlsx
@@ -141,271 +141,271 @@
     <t>card_url_1</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_1_card_1.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_2_card_1.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_3_card_1.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_4_card_1.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_5_card_1.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_6_card_1.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_7_card_1.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_1_card_1.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_2_card_1.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_3_card_1.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_4_card_1.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_5_card_1.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_6_card_1.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_7_card_1.png</t>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_1_card_1.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_2_card_1.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_3_card_1.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_4_card_1.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_5_card_1.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_6_card_1.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_7_card_1.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_1_card_1.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_2_card_1.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_3_card_1.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_4_card_1.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_5_card_1.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_6_card_1.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_7_card_1.png</t>
   </si>
   <si>
     <t>card_url_2</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_1_card_2.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_2_card_2.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_3_card_2.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_4_card_2.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_5_card_2.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_6_card_2.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_7_card_2.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_1_card_2.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_2_card_2.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_3_card_2.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_4_card_2.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_5_card_2.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_6_card_2.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_7_card_2.png</t>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_1_card_2.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_2_card_2.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_3_card_2.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_4_card_2.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_5_card_2.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_6_card_2.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_7_card_2.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_1_card_2.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_2_card_2.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_3_card_2.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_4_card_2.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_5_card_2.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_6_card_2.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_7_card_2.png</t>
   </si>
   <si>
     <t>card_url_3</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_1_card_3.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_2_card_3.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_3_card_3.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_4_card_3.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_5_card_3.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_6_card_3.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_7_card_3.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_1_card_3.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_2_card_3.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_3_card_3.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_4_card_3.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_5_card_3.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_6_card_3.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_7_card_3.png</t>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_1_card_3.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_2_card_3.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_3_card_3.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_4_card_3.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_5_card_3.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_6_card_3.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_7_card_3.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_1_card_3.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_2_card_3.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_3_card_3.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_4_card_3.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_5_card_3.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_6_card_3.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_7_card_3.png</t>
   </si>
   <si>
     <t>card_url_4</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_1_card_4.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_2_card_4.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_3_card_4.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_4_card_4.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_5_card_4.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_6_card_4.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_7_card_4.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_1_card_4.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_2_card_4.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_3_card_4.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_4_card_4.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_5_card_4.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_6_card_4.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_7_card_4.png</t>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_1_card_4.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_2_card_4.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_3_card_4.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_4_card_4.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_5_card_4.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_6_card_4.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_7_card_4.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_1_card_4.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_2_card_4.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_3_card_4.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_4_card_4.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_5_card_4.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_6_card_4.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_7_card_4.png</t>
   </si>
   <si>
     <t>card_url_5</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_1_card_5.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_2_card_5.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_3_card_5.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_4_card_5.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_5_card_5.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_6_card_5.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_7_card_5.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_1_card_5.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_2_card_5.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_3_card_5.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_4_card_5.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_5_card_5.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_6_card_5.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_7_card_5.png</t>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_1_card_5.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_2_card_5.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_3_card_5.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_4_card_5.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_5_card_5.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_6_card_5.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_7_card_5.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_1_card_5.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_2_card_5.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_3_card_5.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_4_card_5.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_5_card_5.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_6_card_5.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_7_card_5.png</t>
   </si>
   <si>
     <t>card_url_6</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_1_card_6.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_2_card_6.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_3_card_6.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_4_card_6.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_5_card_6.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_6_card_6.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/miles_block_7_card_6.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_1_card_6.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_2_card_6.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_3_card_6.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_4_card_6.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_5_card_6.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_6_card_6.png</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/bryanparthum/farmland_conservation/master/images/minutes_block_7_card_6.png</t>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_1_card_6.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_2_card_6.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_3_card_6.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_4_card_6.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_5_card_6.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_6_card_6.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/miles_block_7_card_6.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_1_card_6.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_2_card_6.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_3_card_6.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_4_card_6.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_5_card_6.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_6_card_6.png</t>
+  </si>
+  <si>
+    <t>https://bryanparthum.github.io/farmland_conservation/choice_cards/cards/minutes_block_7_card_6.png</t>
   </si>
   <si>
     <t>card_url_example</t>

</xml_diff>